<commit_message>
Edited code -- By Nirmala
</commit_message>
<xml_diff>
--- a/OrangeHRMDDT/results/TestResults.xlsx
+++ b/OrangeHRMDDT/results/TestResults.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13940" windowHeight="4020"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15390" windowHeight="3195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginValidData" sheetId="1" r:id="rId1"/>
     <sheet name="LoginInvalidData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:J12"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:L9"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -54,16 +54,13 @@
   </si>
   <si>
     <t>Srikoti123!@#</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,7 +84,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -98,11 +95,6 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="17"/>
       </patternFill>
     </fill>
   </fills>
@@ -119,13 +111,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -187,7 +176,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,7 +211,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,28 +388,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.58984375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.26953125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.04296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,37 +420,28 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.65">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -476,21 +456,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.40625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="20.26953125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.2265625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -509,7 +489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -517,7 +497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>